<commit_message>
Cian:  fixed double hashing. TODO: add in collision detection.
</commit_message>
<xml_diff>
--- a/hashmap-excel.xlsx
+++ b/hashmap-excel.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,11 +431,11 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <f>MOD(ABS($B$1*$A6),$B$2)</f>
+        <f t="shared" ref="B6:B22" si="0">MOD(ABS($B$1*$A6),$B$2)</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f>$B$3-(MOD(ABS($A6),$B$3))</f>
+        <f t="shared" ref="C6:C22" si="1">$B$3-(MOD(ABS($A6),$B$3))</f>
         <v>6</v>
       </c>
       <c r="D6">
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G12" si="0">MOD(F6,E6)</f>
+        <f t="shared" ref="G6:G12" si="2">MOD(F6,E6)</f>
         <v>0</v>
       </c>
     </row>
@@ -459,26 +459,26 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <f>MOD(ABS($B$1*$A7),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7">
-        <f>$B$3-(MOD(ABS($A7),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <f>$E$6</f>
+        <f t="shared" ref="E7:E22" si="3">$E$6</f>
         <v>4000</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F12" si="1">B7+D7*C7</f>
+        <f t="shared" ref="F7:F12" si="4">B7+D7*C7</f>
         <v>6</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -487,26 +487,26 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <f>MOD(ABS($B$1*$A8),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8">
-        <f>$B$3-(MOD(ABS($A8),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
@@ -515,26 +515,26 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <f>MOD(ABS($B$1*$A9),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9">
-        <f>$B$3-(MOD(ABS($A9),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -543,26 +543,26 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <f>MOD(ABS($B$1*$A10),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>$B$3-(MOD(ABS($A10),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
     </row>
@@ -571,26 +571,26 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <f>MOD(ABS($B$1*$A11),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C11">
-        <f>$B$3-(MOD(ABS($A11),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
@@ -599,26 +599,26 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <f>MOD(ABS($B$1*$A12),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C12">
-        <f>$B$3-(MOD(ABS($A12),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D12">
         <v>6</v>
       </c>
       <c r="E12">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
@@ -627,26 +627,26 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <f>MOD(ABS($B$1*$A13),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>$B$3-(MOD(ABS($A13),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D13">
         <v>7</v>
       </c>
       <c r="E13">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F17" si="2">B13+D13*C13</f>
+        <f t="shared" ref="F13:F17" si="5">B13+D13*C13</f>
         <v>42</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G17" si="3">MOD(F13,E13)</f>
+        <f t="shared" ref="G13:G17" si="6">MOD(F13,E13)</f>
         <v>42</v>
       </c>
     </row>
@@ -655,18 +655,18 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <f>MOD(ABS($B$1*$A14),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>$B$3-(MOD(ABS($A14),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D14">
         <v>8</v>
       </c>
       <c r="E14">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F14">
@@ -674,64 +674,64 @@
         <v>48</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <f>MOD(ABS($B$1*$A15),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15">
-        <f>$B$3-(MOD(ABS($A15),$B$3))</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>9</v>
       </c>
       <c r="E15">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
-        <v>63</v>
+        <f t="shared" si="5"/>
+        <v>54</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
-        <v>63</v>
+        <f t="shared" si="6"/>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <f>MOD(ABS($B$1*$A16),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>$B$3-(MOD(ABS($A16),$B$3))</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>70</v>
+        <f t="shared" si="5"/>
+        <v>60</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
-        <v>70</v>
+        <f t="shared" si="6"/>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -739,26 +739,26 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <f>MOD(ABS($B$1*$A17),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C17">
-        <f>$B$3-(MOD(ABS($A17),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D17">
         <v>11</v>
       </c>
       <c r="E17">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
     </row>
@@ -767,26 +767,26 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <f>MOD(ABS($B$1*$A18),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>$B$3-(MOD(ABS($A18),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D18">
         <v>12</v>
       </c>
       <c r="E18">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18:F21" si="4">B18+D18*C18</f>
+        <f t="shared" ref="F18:F21" si="7">B18+D18*C18</f>
         <v>72</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G21" si="5">MOD(F18,E18)</f>
+        <f t="shared" ref="G18:G21" si="8">MOD(F18,E18)</f>
         <v>72</v>
       </c>
     </row>
@@ -795,26 +795,26 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <f>MOD(ABS($B$1*$A19),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C19">
-        <f>$B$3-(MOD(ABS($A19),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D19">
         <v>13</v>
       </c>
       <c r="E19">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>78</v>
       </c>
       <c r="G19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>78</v>
       </c>
     </row>
@@ -823,83 +823,83 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <f>MOD(ABS($B$1*$A20),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C20">
-        <f>$B$3-(MOD(ABS($A20),$B$3))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D20">
         <v>14</v>
       </c>
       <c r="E20">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>84</v>
       </c>
       <c r="G20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <f>MOD(ABS($B$1*$A21),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C21">
-        <f>$B$3-(MOD(ABS($A21),$B$3))</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>15</v>
       </c>
       <c r="E21">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
-        <v>105</v>
+        <f t="shared" si="7"/>
+        <v>90</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
-        <v>105</v>
+        <f t="shared" si="8"/>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <f>MOD(ABS($B$1*$A22),$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C22">
-        <f>$B$3-(MOD(ABS($A22),$B$3))</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="D22">
         <v>16</v>
       </c>
       <c r="E22">
-        <f>$E$6</f>
+        <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22" si="6">B22+D22*C22</f>
-        <v>112</v>
+        <f t="shared" ref="F22" si="9">B22+D22*C22</f>
+        <v>96</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22" si="7">MOD(F22,E22)</f>
-        <v>112</v>
+        <f t="shared" ref="G22" si="10">MOD(F22,E22)</f>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cian: completed ChainingHashMap.java.  only partically tested.
</commit_message>
<xml_diff>
--- a/hashmap-excel.xlsx
+++ b/hashmap-excel.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -400,7 +400,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -428,15 +428,15 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <f t="shared" ref="B6:B22" si="0">MOD(ABS($B$1*$A6),$B$2)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C22" si="1">$B$3-(MOD(ABS($A6),$B$3))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -447,11 +447,11 @@
       </c>
       <c r="F6">
         <f>B6+D6*C6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G12" si="2">MOD(F6,E6)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -460,11 +460,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -488,11 +488,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -503,11 +503,11 @@
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -516,11 +516,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -531,11 +531,11 @@
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,11 +544,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -559,11 +559,11 @@
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -572,11 +572,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -587,11 +587,11 @@
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -600,11 +600,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -615,11 +615,11 @@
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -628,11 +628,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -643,11 +643,11 @@
       </c>
       <c r="F13">
         <f t="shared" ref="F13:F17" si="5">B13+D13*C13</f>
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <f t="shared" ref="G13:G17" si="6">MOD(F13,E13)</f>
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -656,11 +656,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -671,11 +671,11 @@
       </c>
       <c r="F14">
         <f>B14+D14*C14</f>
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="G14">
         <f t="shared" si="6"/>
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,11 +684,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -699,11 +699,11 @@
       </c>
       <c r="F15">
         <f t="shared" si="5"/>
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="G15">
         <f t="shared" si="6"/>
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -712,11 +712,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -727,11 +727,11 @@
       </c>
       <c r="F16">
         <f t="shared" si="5"/>
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="G16">
         <f t="shared" si="6"/>
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,11 +740,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -755,11 +755,11 @@
       </c>
       <c r="F17">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="G17">
         <f t="shared" si="6"/>
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -768,11 +768,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -783,11 +783,11 @@
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F21" si="7">B18+D18*C18</f>
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G21" si="8">MOD(F18,E18)</f>
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -796,11 +796,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>13</v>
@@ -811,11 +811,11 @@
       </c>
       <c r="F19">
         <f t="shared" si="7"/>
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="G19">
         <f t="shared" si="8"/>
-        <v>78</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -824,11 +824,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>14</v>
@@ -839,11 +839,11 @@
       </c>
       <c r="F20">
         <f t="shared" si="7"/>
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="G20">
         <f t="shared" si="8"/>
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -852,11 +852,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D21">
         <v>15</v>
@@ -867,11 +867,11 @@
       </c>
       <c r="F21">
         <f t="shared" si="7"/>
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="G21">
         <f t="shared" si="8"/>
-        <v>90</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -880,11 +880,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>16</v>
@@ -895,11 +895,11 @@
       </c>
       <c r="F22">
         <f t="shared" ref="F22" si="9">B22+D22*C22</f>
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22" si="10">MOD(F22,E22)</f>
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cian: fixed up errors for each map, changed something for ChainingHashMap stats (hopefully it is correct now).  Submission 3 to PASTA.
</commit_message>
<xml_diff>
--- a/hashmap-excel.xlsx
+++ b/hashmap-excel.xlsx
@@ -69,12 +69,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +119,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,16 +462,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B22" si="0">MOD(ABS($B$1*$A6),$B$2)</f>
-        <v>4</v>
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" ref="B6:B35" si="0">MOD(ABS($B$1*$A6),$B$2)</f>
+        <v>3</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C22" si="1">$B$3-(MOD(ABS($A6),$B$3))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -447,24 +482,24 @@
       </c>
       <c r="F6">
         <f>B6+D6*C6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G12" si="2">MOD(F6,E6)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -475,24 +510,24 @@
       </c>
       <c r="F7">
         <f t="shared" ref="F7:F12" si="4">B7+D7*C7</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>3</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -503,24 +538,24 @@
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="A9" s="5">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -531,20 +566,20 @@
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>3</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -559,24 +594,24 @@
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -587,24 +622,24 @@
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>3</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -615,24 +650,24 @@
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -643,20 +678,20 @@
       </c>
       <c r="F13">
         <f t="shared" ref="F13:F17" si="5">B13+D13*C13</f>
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G13">
         <f t="shared" ref="G13:G17" si="6">MOD(F13,E13)</f>
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -671,24 +706,24 @@
       </c>
       <c r="F14">
         <f>B14+D14*C14</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <f t="shared" si="6"/>
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="A15" s="3">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -699,24 +734,24 @@
       </c>
       <c r="F15">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G15">
         <f t="shared" si="6"/>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>3</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -727,24 +762,24 @@
       </c>
       <c r="F16">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <f t="shared" si="6"/>
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -755,20 +790,20 @@
       </c>
       <c r="F17">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G17">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="A18" s="4">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -783,24 +818,24 @@
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F21" si="7">B18+D18*C18</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G21" si="8">MOD(F18,E18)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>13</v>
@@ -811,24 +846,24 @@
       </c>
       <c r="F19">
         <f t="shared" si="7"/>
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G19">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="2">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>3</v>
       </c>
       <c r="D20">
         <v>14</v>
@@ -839,24 +874,24 @@
       </c>
       <c r="F20">
         <f t="shared" si="7"/>
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G20">
         <f t="shared" si="8"/>
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>15</v>
@@ -867,20 +902,20 @@
       </c>
       <c r="F21">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="G21">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="A22" s="3">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
@@ -895,11 +930,128 @@
       </c>
       <c r="F22">
         <f t="shared" ref="F22" si="9">B22+D22*C22</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22" si="10">MOD(F22,E22)</f>
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>24</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>26</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>27</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>29</v>
+      </c>
+      <c r="B34" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <f>MOD(ABS($B$1*$A35),$B$2)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>